<commit_message>
prace nad modelem i routami
</commit_message>
<xml_diff>
--- a/ClearanceForm-schema.xlsx
+++ b/ClearanceForm-schema.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\clearanceForm\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
@@ -15,9 +10,9 @@
     <sheet name="methods" sheetId="1" r:id="rId1"/>
     <sheet name="model" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="67">
   <si>
     <t>SysAdmin</t>
   </si>
@@ -223,13 +218,16 @@
   </si>
   <si>
     <t>type: String, enum: ['clearance_unit_managers', 'clearance_unit_admins']</t>
+  </si>
+  <si>
+    <t>notification</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,7 +281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -291,11 +289,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -312,6 +390,27 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -372,7 +471,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -407,7 +506,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -584,28 +683,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -631,10 +730,18 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:15">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="12"/>
       <c r="J2" t="s">
         <v>22</v>
       </c>
@@ -642,190 +749,209 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" t="s">
+    <row r="3" spans="1:15">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="C3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="16"/>
       <c r="O3" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" t="s">
+    <row r="4" spans="1:15">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="C4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="16"/>
       <c r="O4" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" t="s">
+    <row r="5" spans="1:15">
+      <c r="A5" s="13"/>
+      <c r="B5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" t="s">
+      <c r="C5" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="13"/>
+      <c r="B6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" t="s">
+      <c r="C6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="13"/>
+      <c r="B7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" t="s">
+      <c r="C7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="16"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="13"/>
+      <c r="B8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="C8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="16"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A12" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="18"/>
+      <c r="C12" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="20"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -836,30 +962,30 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="H13" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="30">
       <c r="A14" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="D14" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="H14" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="60">
       <c r="A15" s="4" t="s">
         <v>49</v>
       </c>
@@ -867,14 +993,14 @@
         <v>5</v>
       </c>
       <c r="D15" s="5"/>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="30">
       <c r="A16" s="4" t="s">
         <v>57</v>
       </c>
@@ -883,7 +1009,7 @@
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G16" s="9" t="s">
@@ -894,7 +1020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
@@ -903,7 +1029,7 @@
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G17" s="9" t="s">
@@ -911,7 +1037,7 @@
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -920,7 +1046,7 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="30">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
@@ -929,18 +1055,18 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="9" t="s">
         <v>5</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="5"/>
@@ -959,14 +1085,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.5703125" customWidth="1"/>
     <col min="2" max="2" width="68.7109375" customWidth="1"/>
@@ -982,7 +1108,7 @@
     <col min="12" max="12" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -990,7 +1116,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1004,7 +1130,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1018,7 +1144,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="D4" t="s">
         <v>23</v>
       </c>
@@ -1026,7 +1152,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -1037,7 +1163,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1051,7 +1177,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1065,7 +1191,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1079,7 +1205,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1093,67 +1219,67 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>25</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="D13" t="s">
         <v>18</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="D15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1161,32 +1287,32 @@
         <v>21</v>
       </c>
       <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="D17" t="s">
         <v>31</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1194,13 +1320,13 @@
         <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1208,13 +1334,13 @@
         <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1222,13 +1348,13 @@
         <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1236,13 +1362,13 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1250,13 +1376,13 @@
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1264,21 +1390,27 @@
         <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>

</xml_diff>

<commit_message>
working with mongoose objects so a property can be added to this kind of object, reorganization of routes (according to model, not user roles)
</commit_message>
<xml_diff>
--- a/ClearanceForm-schema.xlsx
+++ b/ClearanceForm-schema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="methods" sheetId="1" r:id="rId1"/>
@@ -373,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -411,6 +411,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -683,7 +686,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -693,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -962,7 +965,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="21" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1088,7 +1091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
reorganizing routes, working on tests
</commit_message>
<xml_diff>
--- a/ClearanceForm-schema.xlsx
+++ b/ClearanceForm-schema.xlsx
@@ -686,7 +686,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -984,7 +984,7 @@
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="21" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>